<commit_message>
Made a drop-down list for daycares
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,6 +461,58 @@
         <is>
           <t>foresatt_pnr</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>s2s</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1176187</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>3242</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +700,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,6 +718,17 @@
         <is>
           <t>barn_pnr</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>232323</v>
       </c>
     </row>
   </sheetData>
@@ -679,7 +742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:M1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -749,6 +812,45 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>on</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Sunshine Preschool</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2024-10-24</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>9000000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Oppgave 1 og 2 fullført, mangler å oppdatere antall ledige plasser
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asklo\repo\Oblig5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9FEEC0-C16A-4FBA-819E-A84B6FD08CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA69C8B-6C60-40FA-914C-1922583A0D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4116" yWindow="17172" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>foresatt_id</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>brutto_inntekt</t>
+  </si>
+  <si>
+    <t>svar</t>
   </si>
 </sst>
 </file>
@@ -697,10 +700,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:M1"/>
+  <dimension ref="B1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +721,7 @@
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
@@ -754,6 +757,9 @@
       </c>
       <c r="M1" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>